<commit_message>
Managed the resources in the repo and updated starting board csv file
</commit_message>
<xml_diff>
--- a/ChopShop12x12.xlsx
+++ b/ChopShop12x12.xlsx
@@ -16,9 +16,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>steel 0 0 repair 0 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="42">
+  <si>
+    <t>repair 0 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steel 0 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">repair 0 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pit 0 0 </t>
+  </si>
+  <si>
+    <t>conv 180 1</t>
+  </si>
+  <si>
+    <t>conv 0 1</t>
+  </si>
+  <si>
+    <t>conv 0 2</t>
+  </si>
+  <si>
+    <t>conv 180 2</t>
+  </si>
+  <si>
+    <t>conv 270 2</t>
+  </si>
+  <si>
+    <t>conv 270 1</t>
+  </si>
+  <si>
+    <t>gear 0 1</t>
+  </si>
+  <si>
+    <t>convbr 180 1</t>
+  </si>
+  <si>
+    <t>convbl 180 1</t>
+  </si>
+  <si>
+    <t>convbr 180 2</t>
+  </si>
+  <si>
+    <t>convhr 0 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steel 0 0 laser 0 1  </t>
+  </si>
+  <si>
+    <t>gear 0 0 laser 0 1</t>
+  </si>
+  <si>
+    <t>gear 0 1 laser 0 1</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 270 1</t>
+  </si>
+  <si>
+    <t>conv 0 2 laser 270 1</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 90 1</t>
+  </si>
+  <si>
+    <t>conv 180 1 laser 90 1</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 270 2</t>
+  </si>
+  <si>
+    <t>gear 0 1 laser 270 2</t>
+  </si>
+  <si>
+    <t>gear 0 0 laser 270 2</t>
+  </si>
+  <si>
+    <t>steel 0 0 wall 0 0</t>
+  </si>
+  <si>
+    <t>conv 90 1 wall 0 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 0 1 wall 0 0</t>
+  </si>
+  <si>
+    <t>conv 180 2 laser 270 1 wall 90 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 wall 90 0</t>
+  </si>
+  <si>
+    <t>repair 0 2 wall 90 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 270 2 wall 90 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 0 1  wall 0 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 wall 180 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 0 1 wall 180 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 0 1  wall 180 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 wall 270 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 wall 180 0 wall 270 0</t>
+  </si>
+  <si>
+    <t>convbl 180 1 wall 270 0</t>
+  </si>
+  <si>
+    <t>conv 90 1 wall 270 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 90 1 wall 270 0</t>
+  </si>
+  <si>
+    <t>steel 0 0 laser 270 3 wall 90 0 wall 270 0</t>
   </si>
 </sst>
 </file>
@@ -34,12 +157,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,8 +213,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,19 +516,476 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="30.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="12" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30.75" customHeight="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="50.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>